<commit_message>
Working on model '5 - coupled_model' for testing model integrated solution. Work in progress.
</commit_message>
<xml_diff>
--- a/tests/integration/models/5 - coupled_model/concept.xlsx
+++ b/tests/integration/models/5 - coupled_model/concept.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\pyesm\tests\integration\models\5 - coupled_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B999D9-6318-4485-AB29-83E0AC7C4389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62520A7D-FF90-4B0A-A501-E685454A2864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38490" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -245,8 +245,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="0.0000"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -307,11 +307,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -595,7 +595,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="E4" sqref="E4:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -647,10 +647,10 @@
         <v>2</v>
       </c>
       <c r="E4" s="5">
+        <v>3</v>
+      </c>
+      <c r="F4" s="5">
         <v>0</v>
-      </c>
-      <c r="F4" s="5">
-        <v>10</v>
       </c>
       <c r="I4" t="s">
         <v>38</v>
@@ -690,10 +690,10 @@
         <v>23</v>
       </c>
       <c r="E6" s="6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F6" s="6">
-        <v>1.5</v>
+        <v>10</v>
       </c>
       <c r="I6" t="s">
         <v>39</v>
@@ -736,7 +736,7 @@
       </c>
       <c r="D10">
         <f t="array" ref="D10">MMULT(E4:F4,TRANSPOSE(E5:F5))</f>
-        <v>20</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -829,7 +829,7 @@
         <v>0.9</v>
       </c>
       <c r="F4" s="4">
-        <v>1.194</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="H4" t="s">
         <v>39</v>
@@ -852,7 +852,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="7">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="H5" t="s">
         <v>38</v>

</xml_diff>